<commit_message>
evaluation.py: added safety for standard deviation
</commit_message>
<xml_diff>
--- a/NOTES/job_table_2020.xlsx
+++ b/NOTES/job_table_2020.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t xml:space="preserve">sim_data_cloudMP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSTANT COLL EFFIC=0.5</t>
   </si>
   <si>
     <t xml:space="preserve">solute type</t>
@@ -159,7 +162,7 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,35 +175,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1001</v>
@@ -209,10 +217,10 @@
         <v>1001</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>26</v>
@@ -226,7 +234,7 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1101</v>
@@ -235,10 +243,10 @@
         <v>1101</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>26</v>
@@ -252,7 +260,7 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1201</v>
@@ -261,10 +269,10 @@
         <v>1201</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>26</v>
@@ -278,7 +286,7 @@
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1301</v>
@@ -287,10 +295,10 @@
         <v>1301</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>26</v>
@@ -304,7 +312,7 @@
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>